<commit_message>
Merged windows to dev and updated pipeline
</commit_message>
<xml_diff>
--- a/ProvarProject/templates/AccountData.xlsx
+++ b/ProvarProject/templates/AccountData.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16156\git\ProvarIntegrations\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16156\git\provardx\ProvarProject\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C55A06-E440-42A5-8569-AFCF77470AF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E822A9BC-09B7-49C5-A113-FF05565D5AEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{009709C4-346C-4604-BFFF-F00C948E292F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="NewAccounts" sheetId="1" r:id="rId1"/>
+    <sheet name="VisualforceToLWC" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
   <si>
     <t>AccountName</t>
   </si>
@@ -39,34 +40,52 @@
     <t>Phone</t>
   </si>
   <si>
-    <t>Test1</t>
-  </si>
-  <si>
-    <t>Test2</t>
-  </si>
-  <si>
-    <t>Test3</t>
-  </si>
-  <si>
-    <t>Test4</t>
-  </si>
-  <si>
-    <t>Test5</t>
-  </si>
-  <si>
-    <t>Test6</t>
-  </si>
-  <si>
-    <t>Test7</t>
-  </si>
-  <si>
-    <t>Test8</t>
-  </si>
-  <si>
-    <t>Test9</t>
-  </si>
-  <si>
-    <t>Test10</t>
+    <t>AccountType</t>
+  </si>
+  <si>
+    <t>AccountPhone</t>
+  </si>
+  <si>
+    <t>Employees</t>
+  </si>
+  <si>
+    <t>Edge Communications</t>
+  </si>
+  <si>
+    <t>Customer - Direct</t>
+  </si>
+  <si>
+    <t>Customer - Channel</t>
+  </si>
+  <si>
+    <t>Provar Webinar</t>
+  </si>
+  <si>
+    <t>555-555-5555</t>
+  </si>
+  <si>
+    <t>555-555-5554</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Prospect</t>
+  </si>
+  <si>
+    <t>Channel Partner / Reseller</t>
+  </si>
+  <si>
+    <t>Installation Partner</t>
+  </si>
+  <si>
+    <t>Technology Partner</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>IntegrationTest</t>
   </si>
 </sst>
 </file>
@@ -424,108 +443,267 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F83FDE8E-C72C-491C-8B38-CE5E69B56E5F}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.19921875" customWidth="1"/>
+    <col min="1" max="1" width="17.265625" customWidth="1"/>
+    <col min="2" max="2" width="19.06640625" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <v>5555555501</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>5555555502</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <v>5555555503</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>5555555504</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>5555555505</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B7">
         <v>5555555506</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B8">
         <v>5555555507</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>5555555508</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B10">
         <v>5555555509</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B11">
         <v>5555555510</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>500</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9CA9E5F-E145-47EC-AE0C-D28F5EE988E4}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="11.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>4158563255</v>
+      </c>
+      <c r="D2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>4155554323</v>
+      </c>
+      <c r="D3">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updates to pass ConvertLeadToAccount test case.
Cred update and commented Dreamhouse deployment to Scratch Org.
</commit_message>
<xml_diff>
--- a/ProvarProject/templates/AccountData.xlsx
+++ b/ProvarProject/templates/AccountData.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16156\git\provardx\ProvarProject\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E822A9BC-09B7-49C5-A113-FF05565D5AEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8FBE9B-33BD-463D-8D56-CA44955FB33C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{009709C4-346C-4604-BFFF-F00C948E292F}"/>
+    <workbookView xWindow="-28920" yWindow="4050" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{009709C4-346C-4604-BFFF-F00C948E292F}"/>
   </bookViews>
   <sheets>
     <sheet name="NewAccounts" sheetId="1" r:id="rId1"/>
-    <sheet name="VisualforceToLWC" sheetId="2" r:id="rId2"/>
+    <sheet name="Opp" sheetId="3" r:id="rId2"/>
+    <sheet name="VisualforceToLWC" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
   <si>
     <t>AccountName</t>
   </si>
@@ -86,6 +87,24 @@
   </si>
   <si>
     <t>IntegrationTest</t>
+  </si>
+  <si>
+    <t>OppName</t>
+  </si>
+  <si>
+    <t>Probability</t>
+  </si>
+  <si>
+    <t>Stage</t>
+  </si>
+  <si>
+    <t>CloseDate</t>
+  </si>
+  <si>
+    <t>TestAutomation</t>
+  </si>
+  <si>
+    <t>Needs Analysis</t>
   </si>
 </sst>
 </file>
@@ -445,7 +464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F83FDE8E-C72C-491C-8B38-CE5E69B56E5F}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -618,6 +637,51 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C698D21-FE77-4ADF-BF04-5912E21B384D}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.53125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9CA9E5F-E145-47EC-AE0C-D28F5EE988E4}">
   <dimension ref="A1:D5"/>
   <sheetViews>

</xml_diff>

<commit_message>
Buildkite build file, custom apis, Dreamhouse updates, TM test cases
- Test manager test cases import
- Dreamhouse tests update
- PO operations and custom test steps updates and new files
</commit_message>
<xml_diff>
--- a/ProvarProject/templates/AccountData.xlsx
+++ b/ProvarProject/templates/AccountData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16156\git\provardx\ProvarProject\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8FBE9B-33BD-463D-8D56-CA44955FB33C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FA96CC-3DEE-4D79-80FB-0173F2FFB1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="4050" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{009709C4-346C-4604-BFFF-F00C948E292F}"/>
+    <workbookView xWindow="1837" yWindow="1837" windowWidth="18226" windowHeight="11333" activeTab="1" xr2:uid="{009709C4-346C-4604-BFFF-F00C948E292F}"/>
   </bookViews>
   <sheets>
     <sheet name="NewAccounts" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
   <si>
     <t>AccountName</t>
   </si>
@@ -101,10 +101,31 @@
     <t>CloseDate</t>
   </si>
   <si>
-    <t>TestAutomation</t>
-  </si>
-  <si>
     <t>Needs Analysis</t>
+  </si>
+  <si>
+    <t>TestAutomation1</t>
+  </si>
+  <si>
+    <t>TestAutomation2</t>
+  </si>
+  <si>
+    <t>TestAutomation3</t>
+  </si>
+  <si>
+    <t>TestAutomation4</t>
+  </si>
+  <si>
+    <t>TestAutomation5</t>
+  </si>
+  <si>
+    <t>TestAutomation6</t>
+  </si>
+  <si>
+    <t>TestAutomation7</t>
+  </si>
+  <si>
+    <t>TestAutomation8</t>
   </si>
 </sst>
 </file>
@@ -638,10 +659,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C698D21-FE77-4ADF-BF04-5912E21B384D}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -667,16 +688,94 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>20</v>
       </c>
       <c r="C2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5">
         <v>23</v>
       </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>